<commit_message>
excel data header added
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -15,7 +15,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Stock</t>
+  </si>
   <si>
     <t>asdf</t>
   </si>
@@ -338,30 +350,44 @@
   </sheetViews>
   <sheetData>
     <row r="1">
-      <c r="A1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1">
-        <v>1000</v>
-      </c>
-      <c r="D1">
-        <v>10</v>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2">
       <c r="A2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>1000</v>
       </c>
       <c r="D2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>1000</v>
+      </c>
+      <c r="D3">
         <v>10</v>
       </c>
     </row>

</xml_diff>